<commit_message>
Combo Thermobar and VESical
</commit_message>
<xml_diff>
--- a/docs/Examples/Integration_with_VESIcal/Ol_hosted_melt_inclusions.xlsx
+++ b/docs/Examples/Integration_with_VESIcal/Ol_hosted_melt_inclusions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\OneDrive - Oregon State University\Postdoc\PyMME\MyBarometers\Thermobar_outer\docs\Examples\Integration_with_VESIcal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45D6DE1-C7C5-4D09-A521-16C8DEBFAAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E451F779-94FA-4C4F-A20F-315E2E34946B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{CB67B02E-9E46-4D53-A92F-9499C7F85B2F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{CB67B02E-9E46-4D53-A92F-9499C7F85B2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Ol-Liq" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>Sample number</t>
   </si>
@@ -143,16 +143,31 @@
   </si>
   <si>
     <t>FeOt_Ol</t>
+  </si>
+  <si>
+    <t>Imaginary water-rich sample 1</t>
+  </si>
+  <si>
+    <t>Imaginary water-rich sample 2</t>
+  </si>
+  <si>
+    <t>Imaginary water-rich sample 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -533,7 +548,7 @@
   <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1022,7 +1037,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>10</v>
@@ -1058,7 +1073,7 @@
         <v>0.17599999999999999</v>
       </c>
       <c r="N8" s="3">
-        <v>0.54503033580770699</v>
+        <v>2</v>
       </c>
       <c r="O8" s="3">
         <v>2.0968845746959452E-2</v>
@@ -1090,7 +1105,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>10</v>
@@ -1126,7 +1141,7 @@
         <v>0.184</v>
       </c>
       <c r="N9" s="3">
-        <v>0.53536151893469097</v>
+        <v>4</v>
       </c>
       <c r="O9" s="3">
         <v>2.9343638887944765E-2</v>
@@ -1158,7 +1173,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>10</v>
@@ -1194,7 +1209,7 @@
         <v>0.21199999999999999</v>
       </c>
       <c r="N10" s="3">
-        <v>0.50835172428756426</v>
+        <v>6</v>
       </c>
       <c r="O10" s="3">
         <v>2.5352066632726444E-2</v>
@@ -1222,6 +1237,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>